<commit_message>
Cambio a Flutter 3.35
</commit_message>
<xml_diff>
--- a/Excel/Archivos con ApiHelper.xlsx
+++ b/Excel/Archivos con ApiHelper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Flutter\rowing_app\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB272D8E-1C43-496E-B446-428E9D489A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8C2E6C-B02A-4E4D-A24C-41743DD2AA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{94115EED-1A9C-41CF-A558-7478ADEA294A}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="318">
   <si>
     <t>lib\blocs\location\location_bloc.dart:</t>
   </si>
@@ -96,9 +96,6 @@
     <t>lib\screens\flotas\turnos_agregar_screen.dart:</t>
   </si>
   <si>
-    <t>lib\screens\inicio\home_screen copy.dart:</t>
-  </si>
-  <si>
     <t>lib\screens\inicio\login_screen.dart:</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>lib\screens\obras\veredas_screen.dart:</t>
   </si>
   <si>
-    <t>lib\screens\presentismo\presentismo_screen nuevo.dart:</t>
-  </si>
-  <si>
     <t>lib\screens\presentismo\presentismo_screen.dart:</t>
   </si>
   <si>
@@ -976,6 +970,30 @@
   </si>
   <si>
     <t>  483:     await ApiHelper.post3(/api/Account/ResetPassword', request, widget.token);</t>
+  </si>
+  <si>
+    <t>Elementos en calle</t>
+  </si>
+  <si>
+    <t>Turnos Taller</t>
+  </si>
+  <si>
+    <t>Nuevos Suministros</t>
+  </si>
+  <si>
+    <t>Novedades RRHH</t>
+  </si>
+  <si>
+    <t>Reclamos</t>
+  </si>
+  <si>
+    <t>Veredas</t>
+  </si>
+  <si>
+    <t>Req. de EPP en Seguridad e Higiene</t>
+  </si>
+  <si>
+    <t>Req. de Materiales para una Obra</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1060,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1052,12 +1070,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1190,7 +1202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1206,53 +1218,41 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1605,8 +1605,8 @@
   <dimension ref="A1:X294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1622,22 +1622,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>177</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1646,11 +1646,11 @@
       </c>
       <c r="D2" s="1">
         <f>SUM(D3:D294)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
         <f>+F2-D2</f>
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F2" s="1">
         <f>COUNTBLANK(B1:B294)</f>
@@ -1661,78 +1661,78 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="20">
+      <c r="B3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="16">
         <f>+E2/F2</f>
-        <v>0.9907407407407407</v>
+        <v>0.99537037037037035</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="12" t="s">
-        <v>104</v>
+      <c r="B4" s="14"/>
+      <c r="C4" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="12" t="s">
-        <v>260</v>
+      <c r="B5" s="14"/>
+      <c r="C5" s="8" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="12" t="s">
-        <v>261</v>
+      <c r="B6" s="14"/>
+      <c r="C6" s="8" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="12" t="s">
-        <v>262</v>
+      <c r="B7" s="14"/>
+      <c r="C7" s="8" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="12" t="s">
-        <v>263</v>
+      <c r="B8" s="14"/>
+      <c r="C8" s="8" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="12" t="s">
-        <v>264</v>
+      <c r="B9" s="14"/>
+      <c r="C9" s="8" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="11" t="s">
-        <v>265</v>
+      <c r="B10" s="13"/>
+      <c r="C10" s="7" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1744,38 +1744,38 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>268</v>
+      <c r="B12" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="12" t="s">
-        <v>269</v>
+      <c r="B13" s="14"/>
+      <c r="C13" s="8" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="14" t="s">
-        <v>270</v>
+      <c r="B14" s="14"/>
+      <c r="C14" s="10" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="11" t="s">
-        <v>271</v>
+      <c r="B15" s="13"/>
+      <c r="C15" s="7" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1791,29 +1791,29 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>275</v>
+      <c r="B17" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="12" t="s">
-        <v>276</v>
+      <c r="B18" s="21"/>
+      <c r="C18" s="8" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="11" t="s">
-        <v>277</v>
+      <c r="B19" s="19"/>
+      <c r="C19" s="7" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1831,38 +1831,38 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>273</v>
+      <c r="B21" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="12" t="s">
-        <v>272</v>
+      <c r="B22" s="21"/>
+      <c r="C22" s="8" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="12" t="s">
-        <v>274</v>
+      <c r="B23" s="21"/>
+      <c r="C23" s="8" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="11" t="s">
-        <v>259</v>
+      <c r="B24" s="19"/>
+      <c r="C24" s="7" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1880,47 +1880,47 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>135</v>
+      <c r="B26" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="12" t="s">
-        <v>136</v>
+      <c r="B27" s="14"/>
+      <c r="C27" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="12" t="s">
-        <v>137</v>
+      <c r="B28" s="14"/>
+      <c r="C28" s="8" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="12" t="s">
-        <v>138</v>
+      <c r="B29" s="14"/>
+      <c r="C29" s="8" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="11" t="s">
-        <v>139</v>
+      <c r="B30" s="13"/>
+      <c r="C30" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1932,11 +1932,11 @@
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>134</v>
+      <c r="B32" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1948,92 +1948,92 @@
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>210</v>
+      <c r="B34" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="12" t="s">
-        <v>233</v>
+      <c r="B35" s="14"/>
+      <c r="C35" s="8" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="12" t="s">
-        <v>211</v>
+      <c r="B36" s="14"/>
+      <c r="C36" s="8" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="12" t="s">
-        <v>252</v>
+      <c r="B37" s="14"/>
+      <c r="C37" s="8" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="12" t="s">
-        <v>253</v>
+      <c r="B38" s="14"/>
+      <c r="C38" s="8" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="12" t="s">
-        <v>132</v>
+      <c r="B39" s="14"/>
+      <c r="C39" s="8" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="12" t="s">
-        <v>212</v>
+      <c r="B40" s="14"/>
+      <c r="C40" s="8" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="12" t="s">
-        <v>133</v>
+      <c r="B41" s="14"/>
+      <c r="C41" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="12" t="s">
-        <v>213</v>
+      <c r="B42" s="14"/>
+      <c r="C42" s="8" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="11" t="s">
-        <v>214</v>
+      <c r="B43" s="13"/>
+      <c r="C43" s="7" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2045,38 +2045,38 @@
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>251</v>
+      <c r="B45" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="12" t="s">
-        <v>129</v>
+      <c r="B46" s="14"/>
+      <c r="C46" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="12" t="s">
-        <v>130</v>
+      <c r="B47" s="14"/>
+      <c r="C47" s="8" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="11" t="s">
-        <v>131</v>
+      <c r="B48" s="13"/>
+      <c r="C48" s="7" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -2090,20 +2090,20 @@
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>278</v>
+      <c r="B50" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="11" t="s">
-        <v>279</v>
+      <c r="B51" s="13"/>
+      <c r="C51" s="7" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2119,24 +2119,20 @@
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D53" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="C53" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="11" t="s">
-        <v>254</v>
+      <c r="B54" s="19"/>
+      <c r="C54" s="7" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2154,18 +2150,18 @@
       <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="22" t="s">
-        <v>72</v>
+      <c r="C56" s="18" t="s">
+        <v>70</v>
       </c>
       <c r="D56" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E56" s="24" t="s">
-        <v>283</v>
+      <c r="E56" s="20" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2178,28 +2174,28 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E57" s="24" t="s">
-        <v>284</v>
+      <c r="E57" s="20" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="13" t="s">
-        <v>73</v>
+      <c r="C58" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="11" t="s">
-        <v>255</v>
+      <c r="B59" s="19"/>
+      <c r="C59" s="7" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2217,29 +2213,29 @@
       <c r="A61" s="1">
         <v>60</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="13" t="s">
-        <v>74</v>
+      <c r="C61" s="9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
-      <c r="B62" s="25"/>
-      <c r="C62" s="12" t="s">
-        <v>285</v>
+      <c r="B62" s="21"/>
+      <c r="C62" s="8" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="11" t="s">
-        <v>178</v>
+      <c r="B63" s="13"/>
+      <c r="C63" s="7" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2257,20 +2253,20 @@
       <c r="A65" s="1">
         <v>64</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="13" t="s">
-        <v>75</v>
+      <c r="C65" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
-      <c r="B66" s="23"/>
-      <c r="C66" s="11" t="s">
-        <v>256</v>
+      <c r="B66" s="19"/>
+      <c r="C66" s="7" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2288,38 +2284,38 @@
       <c r="A68" s="1">
         <v>67</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="13" t="s">
-        <v>76</v>
+      <c r="C68" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="12" t="s">
-        <v>179</v>
+      <c r="B69" s="14"/>
+      <c r="C69" s="8" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>69</v>
       </c>
-      <c r="B70" s="18"/>
-      <c r="C70" s="12" t="s">
-        <v>77</v>
+      <c r="B70" s="14"/>
+      <c r="C70" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>70</v>
       </c>
-      <c r="B71" s="17"/>
-      <c r="C71" s="11" t="s">
-        <v>286</v>
+      <c r="B71" s="13"/>
+      <c r="C71" s="7" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2337,65 +2333,65 @@
       <c r="A73" s="1">
         <v>72</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="13" t="s">
-        <v>78</v>
+      <c r="C73" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>73</v>
       </c>
-      <c r="B74" s="18"/>
-      <c r="C74" s="12" t="s">
-        <v>180</v>
+      <c r="B74" s="14"/>
+      <c r="C74" s="8" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>74</v>
       </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="12" t="s">
-        <v>79</v>
+      <c r="B75" s="14"/>
+      <c r="C75" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>75</v>
       </c>
-      <c r="B76" s="18"/>
-      <c r="C76" s="12" t="s">
-        <v>80</v>
+      <c r="B76" s="14"/>
+      <c r="C76" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>76</v>
       </c>
-      <c r="B77" s="18"/>
-      <c r="C77" s="12" t="s">
-        <v>81</v>
+      <c r="B77" s="14"/>
+      <c r="C77" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>77</v>
       </c>
-      <c r="B78" s="18"/>
-      <c r="C78" s="12" t="s">
-        <v>181</v>
+      <c r="B78" s="14"/>
+      <c r="C78" s="8" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>78</v>
       </c>
-      <c r="B79" s="17"/>
-      <c r="C79" s="11" t="s">
-        <v>82</v>
+      <c r="B79" s="13"/>
+      <c r="C79" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2408,20 +2404,20 @@
       <c r="A81" s="1">
         <v>80</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C81" s="13" t="s">
-        <v>83</v>
+      <c r="C81" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>81</v>
       </c>
-      <c r="B82" s="17"/>
-      <c r="C82" s="11" t="s">
-        <v>182</v>
+      <c r="B82" s="13"/>
+      <c r="C82" s="7" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2439,29 +2435,29 @@
       <c r="A84" s="1">
         <v>83</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C84" s="13" t="s">
-        <v>84</v>
+      <c r="C84" s="9" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>84</v>
       </c>
-      <c r="B85" s="18"/>
-      <c r="C85" s="12" t="s">
-        <v>183</v>
+      <c r="B85" s="14"/>
+      <c r="C85" s="8" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>85</v>
       </c>
-      <c r="B86" s="17"/>
-      <c r="C86" s="11" t="s">
-        <v>184</v>
+      <c r="B86" s="13"/>
+      <c r="C86" s="7" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2479,47 +2475,47 @@
       <c r="A88" s="1">
         <v>87</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="B88" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="13" t="s">
-        <v>85</v>
+      <c r="C88" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>88</v>
       </c>
-      <c r="B89" s="18"/>
-      <c r="C89" s="12" t="s">
-        <v>185</v>
+      <c r="B89" s="14"/>
+      <c r="C89" s="8" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>89</v>
       </c>
-      <c r="B90" s="18"/>
-      <c r="C90" s="12" t="s">
-        <v>186</v>
+      <c r="B90" s="14"/>
+      <c r="C90" s="8" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>90</v>
       </c>
-      <c r="B91" s="18"/>
-      <c r="C91" s="12" t="s">
-        <v>187</v>
+      <c r="B91" s="14"/>
+      <c r="C91" s="8" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>91</v>
       </c>
-      <c r="B92" s="17"/>
-      <c r="C92" s="11" t="s">
-        <v>188</v>
+      <c r="B92" s="13"/>
+      <c r="C92" s="7" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2537,41 +2533,41 @@
       <c r="A94" s="1">
         <v>93</v>
       </c>
-      <c r="B94" s="16" t="s">
+      <c r="B94" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C94" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E94" s="26" t="s">
-        <v>296</v>
+      <c r="C94" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E94" s="22" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>94</v>
       </c>
-      <c r="B95" s="18"/>
-      <c r="C95" s="12" t="s">
-        <v>189</v>
+      <c r="B95" s="14"/>
+      <c r="C95" s="8" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>95</v>
       </c>
-      <c r="B96" s="18"/>
-      <c r="C96" s="12" t="s">
-        <v>190</v>
+      <c r="B96" s="14"/>
+      <c r="C96" s="8" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>96</v>
       </c>
-      <c r="B97" s="17"/>
-      <c r="C97" s="11" t="s">
-        <v>87</v>
+      <c r="B97" s="13"/>
+      <c r="C97" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2589,47 +2585,47 @@
       <c r="A99" s="1">
         <v>98</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B99" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C99" s="13" t="s">
-        <v>88</v>
+      <c r="C99" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>99</v>
       </c>
-      <c r="B100" s="18"/>
-      <c r="C100" s="12" t="s">
-        <v>191</v>
+      <c r="B100" s="14"/>
+      <c r="C100" s="8" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>100</v>
       </c>
-      <c r="B101" s="18"/>
-      <c r="C101" s="12" t="s">
-        <v>192</v>
+      <c r="B101" s="14"/>
+      <c r="C101" s="8" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>101</v>
       </c>
-      <c r="B102" s="18"/>
-      <c r="C102" s="12" t="s">
-        <v>193</v>
+      <c r="B102" s="14"/>
+      <c r="C102" s="8" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>102</v>
       </c>
-      <c r="B103" s="17"/>
-      <c r="C103" s="11" t="s">
-        <v>244</v>
+      <c r="B103" s="13"/>
+      <c r="C103" s="7" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2647,11 +2643,11 @@
       <c r="A105" s="1">
         <v>104</v>
       </c>
-      <c r="B105" s="19" t="s">
+      <c r="B105" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C105" s="15" t="s">
-        <v>89</v>
+      <c r="C105" s="11" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2669,83 +2665,83 @@
       <c r="A107" s="1">
         <v>106</v>
       </c>
-      <c r="B107" s="16" t="s">
+      <c r="B107" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C107" s="13" t="s">
-        <v>90</v>
+      <c r="C107" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>107</v>
       </c>
-      <c r="B108" s="25"/>
-      <c r="C108" s="12" t="s">
-        <v>287</v>
+      <c r="B108" s="21"/>
+      <c r="C108" s="8" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>108</v>
       </c>
-      <c r="B109" s="18"/>
-      <c r="C109" s="12" t="s">
-        <v>194</v>
+      <c r="B109" s="14"/>
+      <c r="C109" s="8" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>109</v>
       </c>
-      <c r="B110" s="18"/>
-      <c r="C110" s="12" t="s">
-        <v>91</v>
+      <c r="B110" s="14"/>
+      <c r="C110" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>110</v>
       </c>
-      <c r="B111" s="18"/>
-      <c r="C111" s="12" t="s">
-        <v>288</v>
+      <c r="B111" s="14"/>
+      <c r="C111" s="8" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>111</v>
       </c>
-      <c r="B112" s="18"/>
-      <c r="C112" s="12" t="s">
-        <v>92</v>
+      <c r="B112" s="14"/>
+      <c r="C112" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>112</v>
       </c>
-      <c r="B113" s="18"/>
-      <c r="C113" s="12" t="s">
-        <v>93</v>
+      <c r="B113" s="14"/>
+      <c r="C113" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>113</v>
       </c>
-      <c r="B114" s="18"/>
-      <c r="C114" s="12" t="s">
-        <v>94</v>
+      <c r="B114" s="14"/>
+      <c r="C114" s="8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>114</v>
       </c>
-      <c r="B115" s="17"/>
-      <c r="C115" s="11" t="s">
-        <v>95</v>
+      <c r="B115" s="13"/>
+      <c r="C115" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -2763,47 +2759,47 @@
       <c r="A117" s="1">
         <v>116</v>
       </c>
-      <c r="B117" s="16" t="s">
+      <c r="B117" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C117" s="13" t="s">
-        <v>195</v>
+      <c r="C117" s="9" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>117</v>
       </c>
-      <c r="B118" s="18"/>
-      <c r="C118" s="12" t="s">
-        <v>229</v>
+      <c r="B118" s="14"/>
+      <c r="C118" s="8" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>118</v>
       </c>
-      <c r="B119" s="18"/>
-      <c r="C119" s="12" t="s">
-        <v>96</v>
+      <c r="B119" s="14"/>
+      <c r="C119" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>119</v>
       </c>
-      <c r="B120" s="18"/>
-      <c r="C120" s="12" t="s">
-        <v>97</v>
+      <c r="B120" s="14"/>
+      <c r="C120" s="8" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>120</v>
       </c>
-      <c r="B121" s="17"/>
-      <c r="C121" s="11" t="s">
-        <v>98</v>
+      <c r="B121" s="13"/>
+      <c r="C121" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -2821,29 +2817,29 @@
       <c r="A123" s="1">
         <v>122</v>
       </c>
-      <c r="B123" s="16" t="s">
+      <c r="B123" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C123" s="13" t="s">
-        <v>196</v>
+      <c r="C123" s="9" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>123</v>
       </c>
-      <c r="B124" s="18"/>
-      <c r="C124" s="12" t="s">
-        <v>245</v>
+      <c r="B124" s="14"/>
+      <c r="C124" s="8" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>124</v>
       </c>
-      <c r="B125" s="17"/>
-      <c r="C125" s="11" t="s">
-        <v>246</v>
+      <c r="B125" s="13"/>
+      <c r="C125" s="7" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -2861,29 +2857,29 @@
       <c r="A127" s="1">
         <v>126</v>
       </c>
-      <c r="B127" s="16" t="s">
+      <c r="B127" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C127" s="13" t="s">
-        <v>247</v>
+      <c r="C127" s="9" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>127</v>
       </c>
-      <c r="B128" s="18"/>
-      <c r="C128" s="12" t="s">
-        <v>248</v>
+      <c r="B128" s="14"/>
+      <c r="C128" s="8" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>128</v>
       </c>
-      <c r="B129" s="17"/>
-      <c r="C129" s="11" t="s">
-        <v>197</v>
+      <c r="B129" s="13"/>
+      <c r="C129" s="7" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -2901,23 +2897,23 @@
       <c r="A131" s="1">
         <v>130</v>
       </c>
-      <c r="B131" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="C131" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E131" s="26" t="s">
-        <v>292</v>
+      <c r="B131" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="C131" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E131" s="22" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>131</v>
       </c>
-      <c r="B132" s="17"/>
-      <c r="C132" s="11" t="s">
-        <v>102</v>
+      <c r="B132" s="13"/>
+      <c r="C132" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -2931,32 +2927,32 @@
       <c r="A134" s="1">
         <v>133</v>
       </c>
-      <c r="B134" s="16" t="s">
+      <c r="B134" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C134" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E134" s="24" t="s">
-        <v>291</v>
+      <c r="C134" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E134" s="20" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>134</v>
       </c>
-      <c r="B135" s="25"/>
-      <c r="C135" s="12" t="s">
-        <v>290</v>
+      <c r="B135" s="21"/>
+      <c r="C135" s="8" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>135</v>
       </c>
-      <c r="B136" s="17"/>
-      <c r="C136" s="11" t="s">
-        <v>100</v>
+      <c r="B136" s="13"/>
+      <c r="C136" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -2974,29 +2970,29 @@
       <c r="A138" s="1">
         <v>137</v>
       </c>
-      <c r="B138" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C138" s="13" t="s">
-        <v>198</v>
+      <c r="B138" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C138" s="9" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>138</v>
       </c>
-      <c r="B139" s="18"/>
-      <c r="C139" s="12" t="s">
-        <v>199</v>
+      <c r="B139" s="14"/>
+      <c r="C139" s="8" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>139</v>
       </c>
-      <c r="B140" s="17"/>
-      <c r="C140" s="11" t="s">
-        <v>200</v>
+      <c r="B140" s="13"/>
+      <c r="C140" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -3014,20 +3010,20 @@
       <c r="A142" s="1">
         <v>141</v>
       </c>
-      <c r="B142" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C142" s="13" t="s">
-        <v>201</v>
+      <c r="B142" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C142" s="9" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>142</v>
       </c>
-      <c r="B143" s="17"/>
-      <c r="C143" s="11" t="s">
-        <v>105</v>
+      <c r="B143" s="13"/>
+      <c r="C143" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -3045,47 +3041,47 @@
       <c r="A145" s="1">
         <v>144</v>
       </c>
-      <c r="B145" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C145" s="13" t="s">
-        <v>106</v>
+      <c r="B145" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>145</v>
       </c>
-      <c r="B146" s="18"/>
-      <c r="C146" s="12" t="s">
-        <v>107</v>
+      <c r="B146" s="14"/>
+      <c r="C146" s="8" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>146</v>
       </c>
-      <c r="B147" s="18"/>
-      <c r="C147" s="12" t="s">
-        <v>230</v>
+      <c r="B147" s="14"/>
+      <c r="C147" s="8" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>147</v>
       </c>
-      <c r="B148" s="18"/>
-      <c r="C148" s="12" t="s">
-        <v>108</v>
+      <c r="B148" s="14"/>
+      <c r="C148" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>148</v>
       </c>
-      <c r="B149" s="17"/>
-      <c r="C149" s="11" t="s">
-        <v>109</v>
+      <c r="B149" s="13"/>
+      <c r="C149" s="7" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -3103,11 +3099,11 @@
       <c r="A151" s="1">
         <v>150</v>
       </c>
-      <c r="B151" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C151" s="15" t="s">
-        <v>232</v>
+      <c r="B151" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C151" s="11" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -3125,47 +3121,47 @@
       <c r="A153" s="1">
         <v>152</v>
       </c>
-      <c r="B153" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C153" s="13" t="s">
-        <v>110</v>
+      <c r="B153" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>153</v>
       </c>
-      <c r="B154" s="18"/>
-      <c r="C154" s="12" t="s">
-        <v>111</v>
+      <c r="B154" s="14"/>
+      <c r="C154" s="8" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>154</v>
       </c>
-      <c r="B155" s="18"/>
-      <c r="C155" s="12" t="s">
-        <v>112</v>
+      <c r="B155" s="14"/>
+      <c r="C155" s="8" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>155</v>
       </c>
-      <c r="B156" s="18"/>
-      <c r="C156" s="12" t="s">
-        <v>231</v>
+      <c r="B156" s="14"/>
+      <c r="C156" s="8" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>156</v>
       </c>
-      <c r="B157" s="17"/>
-      <c r="C157" s="11" t="s">
-        <v>113</v>
+      <c r="B157" s="13"/>
+      <c r="C157" s="7" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -3183,11 +3179,11 @@
       <c r="A159" s="1">
         <v>158</v>
       </c>
-      <c r="B159" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="C159" s="15" t="s">
-        <v>298</v>
+      <c r="B159" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="C159" s="11" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -3201,20 +3197,20 @@
       <c r="A161" s="1">
         <v>160</v>
       </c>
-      <c r="B161" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C161" s="13" t="s">
-        <v>202</v>
+      <c r="B161" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>161</v>
       </c>
-      <c r="B162" s="17"/>
-      <c r="C162" s="11" t="s">
-        <v>114</v>
+      <c r="B162" s="13"/>
+      <c r="C162" s="7" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -3232,11 +3228,11 @@
       <c r="A164" s="1">
         <v>163</v>
       </c>
-      <c r="B164" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C164" s="15" t="s">
-        <v>115</v>
+      <c r="B164" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C164" s="11" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -3254,11 +3250,11 @@
       <c r="A166" s="1">
         <v>165</v>
       </c>
-      <c r="B166" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C166" s="15" t="s">
-        <v>116</v>
+      <c r="B166" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C166" s="11" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -3276,11 +3272,11 @@
       <c r="A168" s="1">
         <v>167</v>
       </c>
-      <c r="B168" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C168" s="15" t="s">
-        <v>117</v>
+      <c r="B168" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C168" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -3298,20 +3294,20 @@
       <c r="A170" s="1">
         <v>169</v>
       </c>
-      <c r="B170" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C170" s="13" t="s">
-        <v>118</v>
+      <c r="B170" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C170" s="9" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>170</v>
       </c>
-      <c r="B171" s="17"/>
-      <c r="C171" s="11" t="s">
-        <v>203</v>
+      <c r="B171" s="13"/>
+      <c r="C171" s="7" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -3325,11 +3321,11 @@
       <c r="A173" s="1">
         <v>172</v>
       </c>
-      <c r="B173" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C173" s="15" t="s">
-        <v>119</v>
+      <c r="B173" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C173" s="11" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -3347,20 +3343,20 @@
       <c r="A175" s="1">
         <v>174</v>
       </c>
-      <c r="B175" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C175" s="13" t="s">
-        <v>120</v>
+      <c r="B175" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C175" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>175</v>
       </c>
-      <c r="B176" s="17"/>
-      <c r="C176" s="11" t="s">
-        <v>204</v>
+      <c r="B176" s="13"/>
+      <c r="C176" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -3374,11 +3370,11 @@
       <c r="A178" s="1">
         <v>177</v>
       </c>
-      <c r="B178" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="C178" s="15" t="s">
-        <v>295</v>
+      <c r="B178" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="C178" s="11" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -3396,47 +3392,47 @@
       <c r="A180" s="1">
         <v>179</v>
       </c>
-      <c r="B180" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C180" s="13" t="s">
-        <v>205</v>
+      <c r="B180" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C180" s="9" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>180</v>
       </c>
-      <c r="B181" s="18"/>
-      <c r="C181" s="12" t="s">
-        <v>249</v>
+      <c r="B181" s="14"/>
+      <c r="C181" s="8" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>181</v>
       </c>
-      <c r="B182" s="18"/>
-      <c r="C182" s="12" t="s">
-        <v>121</v>
+      <c r="B182" s="14"/>
+      <c r="C182" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>182</v>
       </c>
-      <c r="B183" s="18"/>
-      <c r="C183" s="12" t="s">
-        <v>250</v>
+      <c r="B183" s="14"/>
+      <c r="C183" s="8" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>183</v>
       </c>
-      <c r="B184" s="17"/>
-      <c r="C184" s="11" t="s">
-        <v>206</v>
+      <c r="B184" s="13"/>
+      <c r="C184" s="7" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -3454,20 +3450,20 @@
       <c r="A186" s="1">
         <v>185</v>
       </c>
-      <c r="B186" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C186" s="13" t="s">
-        <v>122</v>
+      <c r="B186" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C186" s="9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>186</v>
       </c>
-      <c r="B187" s="17"/>
-      <c r="C187" s="11" t="s">
-        <v>123</v>
+      <c r="B187" s="13"/>
+      <c r="C187" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
@@ -3485,11 +3481,11 @@
       <c r="A189" s="1">
         <v>188</v>
       </c>
-      <c r="B189" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C189" s="15" t="s">
-        <v>124</v>
+      <c r="B189" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C189" s="11" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
@@ -3507,23 +3503,23 @@
       <c r="A191" s="1">
         <v>190</v>
       </c>
-      <c r="B191" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C191" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="E191" s="26" t="s">
-        <v>293</v>
+      <c r="B191" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C191" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E191" s="22" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>191</v>
       </c>
-      <c r="B192" s="17"/>
-      <c r="C192" s="11" t="s">
-        <v>125</v>
+      <c r="B192" s="13"/>
+      <c r="C192" s="7" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -3541,29 +3537,29 @@
       <c r="A194" s="1">
         <v>193</v>
       </c>
-      <c r="B194" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C194" s="13" t="s">
-        <v>126</v>
+      <c r="B194" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C194" s="9" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>194</v>
       </c>
-      <c r="B195" s="18"/>
-      <c r="C195" s="12" t="s">
-        <v>127</v>
+      <c r="B195" s="14"/>
+      <c r="C195" s="8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>195</v>
       </c>
-      <c r="B196" s="17"/>
-      <c r="C196" s="11" t="s">
-        <v>208</v>
+      <c r="B196" s="13"/>
+      <c r="C196" s="7" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
@@ -3581,20 +3577,20 @@
       <c r="A198" s="1">
         <v>197</v>
       </c>
-      <c r="B198" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C198" s="13" t="s">
-        <v>128</v>
+      <c r="B198" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C198" s="9" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>198</v>
       </c>
-      <c r="B199" s="17"/>
-      <c r="C199" s="11" t="s">
-        <v>209</v>
+      <c r="B199" s="13"/>
+      <c r="C199" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
@@ -3612,41 +3608,41 @@
       <c r="A201" s="1">
         <v>200</v>
       </c>
-      <c r="B201" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C201" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="E201" s="26" t="s">
-        <v>299</v>
+      <c r="B201" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C201" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E201" s="22" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>201</v>
       </c>
-      <c r="B202" s="18"/>
-      <c r="C202" s="12" t="s">
-        <v>141</v>
+      <c r="B202" s="14"/>
+      <c r="C202" s="8" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>202</v>
       </c>
-      <c r="B203" s="18"/>
-      <c r="C203" s="12" t="s">
-        <v>142</v>
+      <c r="B203" s="14"/>
+      <c r="C203" s="8" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>203</v>
       </c>
-      <c r="B204" s="17"/>
-      <c r="C204" s="11" t="s">
-        <v>143</v>
+      <c r="B204" s="13"/>
+      <c r="C204" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -3664,29 +3660,29 @@
       <c r="A206" s="1">
         <v>205</v>
       </c>
-      <c r="B206" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C206" s="13" t="s">
-        <v>144</v>
+      <c r="B206" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C206" s="9" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>206</v>
       </c>
-      <c r="B207" s="18"/>
-      <c r="C207" s="12" t="s">
-        <v>215</v>
+      <c r="B207" s="14"/>
+      <c r="C207" s="8" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>207</v>
       </c>
-      <c r="B208" s="17"/>
-      <c r="C208" s="11" t="s">
-        <v>145</v>
+      <c r="B208" s="13"/>
+      <c r="C208" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
@@ -3704,23 +3700,23 @@
       <c r="A210" s="1">
         <v>209</v>
       </c>
-      <c r="B210" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C210" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="E210" s="26" t="s">
-        <v>300</v>
+      <c r="B210" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C210" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E210" s="22" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>210</v>
       </c>
-      <c r="B211" s="17"/>
-      <c r="C211" s="11" t="s">
-        <v>146</v>
+      <c r="B211" s="13"/>
+      <c r="C211" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
@@ -3738,56 +3734,56 @@
       <c r="A213" s="1">
         <v>212</v>
       </c>
-      <c r="B213" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C213" s="13" t="s">
-        <v>147</v>
+      <c r="B213" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C213" s="9" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>213</v>
       </c>
-      <c r="B214" s="18"/>
-      <c r="C214" s="12" t="s">
-        <v>148</v>
+      <c r="B214" s="14"/>
+      <c r="C214" s="8" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>214</v>
       </c>
-      <c r="B215" s="18"/>
-      <c r="C215" s="12" t="s">
-        <v>149</v>
+      <c r="B215" s="14"/>
+      <c r="C215" s="8" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>215</v>
       </c>
-      <c r="B216" s="18"/>
-      <c r="C216" s="12" t="s">
-        <v>150</v>
+      <c r="B216" s="14"/>
+      <c r="C216" s="8" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>216</v>
       </c>
-      <c r="B217" s="18"/>
-      <c r="C217" s="12" t="s">
-        <v>151</v>
+      <c r="B217" s="14"/>
+      <c r="C217" s="8" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>217</v>
       </c>
-      <c r="B218" s="17"/>
-      <c r="C218" s="11" t="s">
-        <v>237</v>
+      <c r="B218" s="13"/>
+      <c r="C218" s="7" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
@@ -3801,47 +3797,47 @@
       <c r="A220" s="1">
         <v>219</v>
       </c>
-      <c r="B220" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C220" s="13" t="s">
-        <v>238</v>
+      <c r="B220" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C220" s="9" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>220</v>
       </c>
-      <c r="B221" s="18"/>
-      <c r="C221" s="12" t="s">
-        <v>152</v>
+      <c r="B221" s="14"/>
+      <c r="C221" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>221</v>
       </c>
-      <c r="B222" s="18"/>
-      <c r="C222" s="12" t="s">
-        <v>153</v>
+      <c r="B222" s="14"/>
+      <c r="C222" s="8" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>222</v>
       </c>
-      <c r="B223" s="18"/>
-      <c r="C223" s="12" t="s">
-        <v>154</v>
+      <c r="B223" s="14"/>
+      <c r="C223" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>223</v>
       </c>
-      <c r="B224" s="17"/>
-      <c r="C224" s="11" t="s">
-        <v>217</v>
+      <c r="B224" s="13"/>
+      <c r="C224" s="7" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -3855,11 +3851,11 @@
       <c r="A226" s="1">
         <v>225</v>
       </c>
-      <c r="B226" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C226" s="15" t="s">
-        <v>239</v>
+      <c r="B226" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C226" s="11" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -3873,20 +3869,20 @@
       <c r="A228" s="1">
         <v>227</v>
       </c>
-      <c r="B228" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C228" s="13" t="s">
-        <v>218</v>
+      <c r="B228" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C228" s="9" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>228</v>
       </c>
-      <c r="B229" s="23"/>
-      <c r="C229" s="11" t="s">
-        <v>309</v>
+      <c r="B229" s="19"/>
+      <c r="C229" s="7" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -3904,20 +3900,20 @@
       <c r="A231" s="1">
         <v>230</v>
       </c>
-      <c r="B231" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="C231" s="13" t="s">
-        <v>302</v>
+      <c r="B231" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C231" s="9" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>231</v>
       </c>
-      <c r="B232" s="17"/>
-      <c r="C232" s="11" t="s">
-        <v>219</v>
+      <c r="B232" s="13"/>
+      <c r="C232" s="7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
@@ -3931,11 +3927,11 @@
       <c r="A234" s="1">
         <v>233</v>
       </c>
-      <c r="B234" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C234" s="15" t="s">
-        <v>240</v>
+      <c r="B234" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C234" s="11" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
@@ -3949,11 +3945,11 @@
       <c r="A236" s="1">
         <v>235</v>
       </c>
-      <c r="B236" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="C236" s="15" t="s">
-        <v>304</v>
+      <c r="B236" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="C236" s="11" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
@@ -3971,38 +3967,38 @@
       <c r="A238" s="1">
         <v>237</v>
       </c>
-      <c r="B238" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C238" s="13" t="s">
-        <v>155</v>
+      <c r="B238" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C238" s="9" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>238</v>
       </c>
-      <c r="B239" s="18"/>
-      <c r="C239" s="12" t="s">
-        <v>156</v>
+      <c r="B239" s="14"/>
+      <c r="C239" s="8" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>239</v>
       </c>
-      <c r="B240" s="18"/>
-      <c r="C240" s="12" t="s">
-        <v>311</v>
+      <c r="B240" s="14"/>
+      <c r="C240" s="8" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>240</v>
       </c>
-      <c r="B241" s="17"/>
-      <c r="C241" s="11" t="s">
-        <v>310</v>
+      <c r="B241" s="13"/>
+      <c r="C241" s="7" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
@@ -4020,20 +4016,20 @@
       <c r="A243" s="1">
         <v>242</v>
       </c>
-      <c r="B243" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C243" s="13" t="s">
-        <v>157</v>
+      <c r="B243" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C243" s="9" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>243</v>
       </c>
-      <c r="B244" s="17"/>
-      <c r="C244" s="11" t="s">
-        <v>158</v>
+      <c r="B244" s="13"/>
+      <c r="C244" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
@@ -4047,20 +4043,20 @@
       <c r="A246" s="1">
         <v>245</v>
       </c>
-      <c r="B246" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C246" s="13" t="s">
-        <v>159</v>
+      <c r="B246" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C246" s="9" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>246</v>
       </c>
-      <c r="B247" s="17"/>
-      <c r="C247" s="11" t="s">
-        <v>241</v>
+      <c r="B247" s="13"/>
+      <c r="C247" s="7" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
@@ -4074,14 +4070,14 @@
       <c r="A249" s="1">
         <v>248</v>
       </c>
-      <c r="B249" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C249" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E249" s="26" t="s">
-        <v>308</v>
+      <c r="B249" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C249" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E249" s="22" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
@@ -4099,20 +4095,20 @@
       <c r="A251" s="1">
         <v>250</v>
       </c>
-      <c r="B251" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C251" s="13" t="s">
-        <v>161</v>
+      <c r="B251" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C251" s="9" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>251</v>
       </c>
-      <c r="B252" s="17"/>
-      <c r="C252" s="11" t="s">
-        <v>162</v>
+      <c r="B252" s="13"/>
+      <c r="C252" s="7" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
@@ -4130,11 +4126,11 @@
       <c r="A254" s="1">
         <v>253</v>
       </c>
-      <c r="B254" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C254" s="15" t="s">
-        <v>220</v>
+      <c r="B254" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C254" s="11" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
@@ -4152,11 +4148,11 @@
       <c r="A256" s="1">
         <v>255</v>
       </c>
-      <c r="B256" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C256" s="15" t="s">
-        <v>221</v>
+      <c r="B256" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C256" s="11" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="257" spans="1:24" x14ac:dyDescent="0.2">
@@ -4174,33 +4170,33 @@
       <c r="A258" s="1">
         <v>257</v>
       </c>
-      <c r="B258" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C258" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="E258" s="28" t="s">
-        <v>305</v>
-      </c>
-      <c r="G258" s="27"/>
-      <c r="H258" s="27"/>
-      <c r="I258" s="27"/>
-      <c r="J258" s="27"/>
-      <c r="K258" s="27"/>
-      <c r="L258" s="27"/>
-      <c r="M258" s="27"/>
-      <c r="N258" s="27"/>
-      <c r="O258" s="27"/>
-      <c r="P258" s="27"/>
-      <c r="Q258" s="27"/>
-      <c r="R258" s="27"/>
-      <c r="S258" s="27"/>
-      <c r="T258" s="27"/>
-      <c r="U258" s="27"/>
-      <c r="V258" s="27"/>
-      <c r="W258" s="27"/>
-      <c r="X258" s="27"/>
+      <c r="B258" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C258" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E258" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="G258" s="23"/>
+      <c r="H258" s="23"/>
+      <c r="I258" s="23"/>
+      <c r="J258" s="23"/>
+      <c r="K258" s="23"/>
+      <c r="L258" s="23"/>
+      <c r="M258" s="23"/>
+      <c r="N258" s="23"/>
+      <c r="O258" s="23"/>
+      <c r="P258" s="23"/>
+      <c r="Q258" s="23"/>
+      <c r="R258" s="23"/>
+      <c r="S258" s="23"/>
+      <c r="T258" s="23"/>
+      <c r="U258" s="23"/>
+      <c r="V258" s="23"/>
+      <c r="W258" s="23"/>
+      <c r="X258" s="23"/>
     </row>
     <row r="259" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
@@ -4217,50 +4213,50 @@
       <c r="A260" s="1">
         <v>259</v>
       </c>
-      <c r="B260" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C260" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E260" s="26" t="s">
-        <v>299</v>
+      <c r="B260" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C260" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E260" s="22" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="261" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>260</v>
       </c>
-      <c r="B261" s="18"/>
-      <c r="C261" s="12" t="s">
-        <v>165</v>
+      <c r="B261" s="14"/>
+      <c r="C261" s="8" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="262" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>261</v>
       </c>
-      <c r="B262" s="18"/>
-      <c r="C262" s="12" t="s">
-        <v>166</v>
+      <c r="B262" s="14"/>
+      <c r="C262" s="8" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="263" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>262</v>
       </c>
-      <c r="B263" s="18"/>
-      <c r="C263" s="12" t="s">
-        <v>167</v>
+      <c r="B263" s="14"/>
+      <c r="C263" s="8" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="264" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>263</v>
       </c>
-      <c r="B264" s="17"/>
-      <c r="C264" s="11" t="s">
-        <v>168</v>
+      <c r="B264" s="13"/>
+      <c r="C264" s="7" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="265" spans="1:24" x14ac:dyDescent="0.2">
@@ -4278,20 +4274,20 @@
       <c r="A266" s="1">
         <v>265</v>
       </c>
-      <c r="B266" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C266" s="13" t="s">
-        <v>169</v>
+      <c r="B266" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C266" s="9" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="267" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>266</v>
       </c>
-      <c r="B267" s="17"/>
-      <c r="C267" s="11" t="s">
-        <v>222</v>
+      <c r="B267" s="13"/>
+      <c r="C267" s="7" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="268" spans="1:24" x14ac:dyDescent="0.2">
@@ -4309,11 +4305,11 @@
       <c r="A269" s="1">
         <v>268</v>
       </c>
-      <c r="B269" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C269" s="15" t="s">
-        <v>223</v>
+      <c r="B269" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C269" s="11" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="270" spans="1:24" x14ac:dyDescent="0.2">
@@ -4327,11 +4323,11 @@
       <c r="A271" s="1">
         <v>270</v>
       </c>
-      <c r="B271" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C271" s="15" t="s">
-        <v>242</v>
+      <c r="B271" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C271" s="11" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="272" spans="1:24" x14ac:dyDescent="0.2">
@@ -4345,47 +4341,47 @@
       <c r="A273" s="1">
         <v>272</v>
       </c>
-      <c r="B273" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C273" s="13" t="s">
-        <v>224</v>
+      <c r="B273" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C273" s="9" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>273</v>
       </c>
-      <c r="B274" s="18"/>
-      <c r="C274" s="12" t="s">
-        <v>225</v>
+      <c r="B274" s="14"/>
+      <c r="C274" s="8" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>274</v>
       </c>
-      <c r="B275" s="18"/>
-      <c r="C275" s="12" t="s">
-        <v>243</v>
+      <c r="B275" s="14"/>
+      <c r="C275" s="8" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>275</v>
       </c>
-      <c r="B276" s="18"/>
-      <c r="C276" s="12" t="s">
-        <v>226</v>
+      <c r="B276" s="14"/>
+      <c r="C276" s="8" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>276</v>
       </c>
-      <c r="B277" s="17"/>
-      <c r="C277" s="11" t="s">
-        <v>236</v>
+      <c r="B277" s="13"/>
+      <c r="C277" s="7" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.2">
@@ -4399,20 +4395,20 @@
       <c r="A279" s="1">
         <v>278</v>
       </c>
-      <c r="B279" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C279" s="13" t="s">
-        <v>170</v>
+      <c r="B279" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C279" s="9" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>279</v>
       </c>
-      <c r="B280" s="17"/>
-      <c r="C280" s="11" t="s">
-        <v>235</v>
+      <c r="B280" s="13"/>
+      <c r="C280" s="7" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.2">
@@ -4430,11 +4426,11 @@
       <c r="A282" s="1">
         <v>281</v>
       </c>
-      <c r="B282" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C282" s="15" t="s">
-        <v>171</v>
+      <c r="B282" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C282" s="11" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.2">
@@ -4452,32 +4448,32 @@
       <c r="A284" s="1">
         <v>283</v>
       </c>
-      <c r="B284" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C284" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="E284" s="26" t="s">
-        <v>306</v>
+      <c r="B284" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C284" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E284" s="22" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>284</v>
       </c>
-      <c r="B285" s="18"/>
-      <c r="C285" s="12" t="s">
-        <v>228</v>
+      <c r="B285" s="14"/>
+      <c r="C285" s="8" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>285</v>
       </c>
-      <c r="B286" s="17"/>
-      <c r="C286" s="11" t="s">
-        <v>266</v>
+      <c r="B286" s="13"/>
+      <c r="C286" s="7" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.2">
@@ -4491,11 +4487,11 @@
       <c r="A288" s="1">
         <v>287</v>
       </c>
-      <c r="B288" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C288" s="15" t="s">
-        <v>234</v>
+      <c r="B288" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C288" s="11" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
@@ -4513,29 +4509,29 @@
       <c r="A290" s="1">
         <v>289</v>
       </c>
-      <c r="B290" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C290" s="13" t="s">
-        <v>172</v>
+      <c r="B290" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C290" s="9" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>290</v>
       </c>
-      <c r="B291" s="18"/>
-      <c r="C291" s="12" t="s">
-        <v>173</v>
+      <c r="B291" s="14"/>
+      <c r="C291" s="8" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>291</v>
       </c>
-      <c r="B292" s="17"/>
-      <c r="C292" s="11" t="s">
-        <v>174</v>
+      <c r="B292" s="13"/>
+      <c r="C292" s="7" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
@@ -4553,11 +4549,11 @@
       <c r="A294" s="1">
         <v>293</v>
       </c>
-      <c r="B294" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C294" s="15" t="s">
-        <v>307</v>
+      <c r="B294" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C294" s="11" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -4569,381 +4565,256 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9322231A-3280-48FF-912F-3416124A4DDC}">
-  <dimension ref="A1:A72"/>
+  <dimension ref="A1:A74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>176</v>
+      <c r="A1" s="22" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
+      <c r="A2" s="22" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
+      <c r="A3" s="22" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>2</v>
+      <c r="A4" s="22" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>3</v>
+      <c r="A5" s="22" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>4</v>
+      <c r="A6" s="22" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>5</v>
+      <c r="A7" s="22" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>6</v>
+      <c r="A8" s="22" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>17</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="A21" s="1"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="A24" s="1"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="A25" s="1"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="A27" s="1"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="A28" s="1"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="A29" s="1"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="A30" s="1"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>31</v>
-      </c>
+      <c r="A33" s="1"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="A34" s="1"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="A35" s="1"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="A36" s="1"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A37" s="1"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="A38" s="1"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="A39" s="1"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="A42" s="1"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
-        <v>41</v>
-      </c>
+      <c r="A43" s="1"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="A44" s="1"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="A45" s="1"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="A46" s="1"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="A47" s="1"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
-        <v>46</v>
-      </c>
+      <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="A49" s="1"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="9" t="s">
-        <v>48</v>
-      </c>
+      <c r="A50" s="1"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
-        <v>49</v>
-      </c>
+      <c r="A51" s="1"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A52" s="1"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="A53" s="1"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
-        <v>52</v>
-      </c>
+      <c r="A54" s="1"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="A55" s="1"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A56" s="1"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="A58" s="1"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="9" t="s">
-        <v>57</v>
-      </c>
+      <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="A60" s="1"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="A61" s="1"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="A62" s="1"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="9" t="s">
-        <v>61</v>
-      </c>
+      <c r="A63" s="1"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="9" t="s">
-        <v>62</v>
-      </c>
+      <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="A65" s="1"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="A66" s="1"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="A67" s="1"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="9" t="s">
-        <v>66</v>
-      </c>
+      <c r="A68" s="1"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="9" t="s">
-        <v>67</v>
-      </c>
+      <c r="A69" s="1"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="9" t="s">
-        <v>68</v>
-      </c>
+      <c r="A70" s="1"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="9" t="s">
-        <v>69</v>
-      </c>
+      <c r="A71" s="1"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="9" t="s">
-        <v>70</v>
-      </c>
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A72">
-    <sortCondition ref="A1:A72"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>